<commit_message>
Added all results from all experiments in xlsx format
</commit_message>
<xml_diff>
--- a/experiments_results/[1] FracFactDesign_ANOVA_results.xlsx
+++ b/experiments_results/[1] FracFactDesign_ANOVA_results.xlsx
@@ -495,16 +495,16 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>16143.84375003111</v>
+        <v>0.825</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2">
-        <v>256.0966380094064</v>
+        <v>0.263</v>
       </c>
       <c r="E2">
-        <v>5.75542616550835E-09</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -512,16 +512,16 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>99.6201412812471</v>
+        <v>4.692</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>1.580316537695696</v>
+        <v>1.498</v>
       </c>
       <c r="E3">
-        <v>0.2347515478317453</v>
+        <v>0.252</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -529,16 +529,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>228.5575450312468</v>
+        <v>4524.858</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4">
-        <v>3.62570523974955</v>
+        <v>1444.132</v>
       </c>
       <c r="E4">
-        <v>0.08336574309789743</v>
+        <v>3.003321566616797E-11</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -546,16 +546,16 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>27789.32593828123</v>
+        <v>44046.367</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5">
-        <v>440.8338593668377</v>
+        <v>14057.622</v>
       </c>
       <c r="E5">
-        <v>3.170918068667451E-10</v>
+        <v>1.09680721783061E-15</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -563,16 +563,16 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>36829.86205528129</v>
+        <v>5105.875</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6">
-        <v>584.2477167613547</v>
+        <v>1629.566</v>
       </c>
       <c r="E6">
-        <v>6.94436184493161E-11</v>
+        <v>1.748885486397493E-11</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -580,16 +580,16 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>113.089520281249</v>
+        <v>0.01237164500000661</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7">
-        <v>1.793987007466462</v>
+        <v>0.003948473566969992</v>
       </c>
       <c r="E7">
-        <v>0.2074581682557766</v>
+        <v>0.951</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -597,16 +597,16 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>314.5596325312478</v>
+        <v>75.857</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8">
-        <v>4.98999281658506</v>
+        <v>24.21</v>
       </c>
       <c r="E8">
-        <v>0.04720877698886222</v>
+        <v>0.000824185498638506</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -614,16 +614,16 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>113.0895202812507</v>
+        <v>0.01237164500000884</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9">
-        <v>1.793987007466489</v>
+        <v>0.003948473566970702</v>
       </c>
       <c r="E9">
-        <v>0.2074581682557735</v>
+        <v>0.951</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -631,16 +631,16 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <v>314.5596325312532</v>
+        <v>1.13</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10">
-        <v>4.989992816585145</v>
+        <v>0.361</v>
       </c>
       <c r="E10">
-        <v>0.04720877698886065</v>
+        <v>0.5629999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -648,16 +648,16 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>13015.98350403126</v>
+        <v>1.661</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11">
-        <v>206.4780647893643</v>
+        <v>0.53</v>
       </c>
       <c r="E11">
-        <v>1.789648335231749E-08</v>
+        <v>0.485</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -665,16 +665,16 @@
         <v>14</v>
       </c>
       <c r="B12">
-        <v>567.3817195312517</v>
+        <v>5.378</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12">
-        <v>9.000616773168998</v>
+        <v>1.716</v>
       </c>
       <c r="E12">
-        <v>0.012077620325608</v>
+        <v>0.223</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -682,16 +682,16 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>99.62014128124621</v>
+        <v>4.692</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13">
-        <v>1.580316537695682</v>
+        <v>1.498</v>
       </c>
       <c r="E13">
-        <v>0.2347515478317473</v>
+        <v>0.252</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -699,16 +699,16 @@
         <v>16</v>
       </c>
       <c r="B14">
-        <v>228.5575450312508</v>
+        <v>7.265</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14">
-        <v>3.625705239749612</v>
+        <v>2.319</v>
       </c>
       <c r="E14">
-        <v>0.08336574309789509</v>
+        <v>0.162</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -716,16 +716,16 @@
         <v>17</v>
       </c>
       <c r="B15">
-        <v>26.5483627812502</v>
+        <v>0.714</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15">
-        <v>0.421147934668231</v>
+        <v>0.228</v>
       </c>
       <c r="E15">
-        <v>0.5296808495388906</v>
+        <v>0.644</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -733,16 +733,16 @@
         <v>18</v>
       </c>
       <c r="B16">
-        <v>42.33610153125023</v>
+        <v>4.481</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16">
-        <v>0.6715955280821627</v>
+        <v>1.43</v>
       </c>
       <c r="E16">
-        <v>0.42989467913168</v>
+        <v>0.262</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -750,16 +750,16 @@
         <v>19</v>
       </c>
       <c r="B17">
-        <v>1.26047503125027</v>
+        <v>5.59</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17">
-        <v>0.01999544983191339</v>
+        <v>1.784</v>
       </c>
       <c r="E17">
-        <v>0.8901062373506773</v>
+        <v>0.214</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -767,16 +767,16 @@
         <v>20</v>
       </c>
       <c r="B18">
-        <v>16143.84375003136</v>
+        <v>0.825</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18">
-        <v>256.0966380094103</v>
+        <v>0.263</v>
       </c>
       <c r="E18">
-        <v>5.755426165507896E-09</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -784,16 +784,16 @@
         <v>21</v>
       </c>
       <c r="B19">
-        <v>13.20851503124997</v>
+        <v>4.69</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19">
-        <v>0.2095322740343858</v>
+        <v>1.497</v>
       </c>
       <c r="E19">
-        <v>0.6560435775647565</v>
+        <v>0.252</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -801,16 +801,16 @@
         <v>22</v>
       </c>
       <c r="B20">
-        <v>133.608117781248</v>
+        <v>4526.381</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20">
-        <v>2.119482219002303</v>
+        <v>1444.617</v>
       </c>
       <c r="E20">
-        <v>0.1733761546371787</v>
+        <v>2.998804759619007E-11</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -818,16 +818,16 @@
         <v>23</v>
       </c>
       <c r="B21">
-        <v>61.17562578124787</v>
+        <v>54.08</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21">
-        <v>0.9704548887664347</v>
+        <v>17.26</v>
       </c>
       <c r="E21">
-        <v>0.3457393282976391</v>
+        <v>0.002467793261966397</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -835,16 +835,16 @@
         <v>24</v>
       </c>
       <c r="B22">
-        <v>13.20851503125052</v>
+        <v>6.529</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22">
-        <v>0.2095322740343945</v>
+        <v>2.084</v>
       </c>
       <c r="E22">
-        <v>0.6560435775647497</v>
+        <v>0.183</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -852,16 +852,16 @@
         <v>25</v>
       </c>
       <c r="B23">
-        <v>16143.84375003138</v>
+        <v>5025.071</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23">
-        <v>256.0966380094106</v>
+        <v>1603.777</v>
       </c>
       <c r="E23">
-        <v>5.755426165507853E-09</v>
+        <v>1.878365315325018E-11</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -869,16 +869,16 @@
         <v>26</v>
       </c>
       <c r="B24">
-        <v>1342.228719031259</v>
+        <v>5025.071</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24">
-        <v>21.2923432427866</v>
+        <v>1603.777</v>
       </c>
       <c r="E24">
-        <v>0.000747208851696936</v>
+        <v>1.878365315325036E-11</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -886,16 +886,16 @@
         <v>27</v>
       </c>
       <c r="B25">
-        <v>34.79239653125076</v>
+        <v>0.435</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25">
-        <v>0.5519265373171294</v>
+        <v>0.139</v>
       </c>
       <c r="E25">
-        <v>0.4730995619470187</v>
+        <v>0.718</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -903,16 +903,16 @@
         <v>28</v>
       </c>
       <c r="B26">
-        <v>169.0362877812522</v>
+        <v>54.08</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
       <c r="D26">
-        <v>2.681494300406974</v>
+        <v>17.26</v>
       </c>
       <c r="E26">
-        <v>0.1297812506971127</v>
+        <v>0.002467793261966397</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -920,16 +920,16 @@
         <v>29</v>
       </c>
       <c r="B27">
-        <v>7.128144031249875</v>
+        <v>0.11</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
       <c r="D27">
-        <v>0.1130767709298718</v>
+        <v>0.03499613678177024</v>
       </c>
       <c r="E27">
-        <v>0.7429953622872929</v>
+        <v>0.856</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -937,16 +937,16 @@
         <v>30</v>
       </c>
       <c r="B28">
-        <v>46.18806328125029</v>
+        <v>4526.381</v>
       </c>
       <c r="C28">
         <v>1</v>
       </c>
       <c r="D28">
-        <v>0.7327008304618358</v>
+        <v>1444.617</v>
       </c>
       <c r="E28">
-        <v>0.4102677114079503</v>
+        <v>2.998804759619067E-11</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -954,16 +954,16 @@
         <v>31</v>
       </c>
       <c r="B29">
-        <v>26.54836278124792</v>
+        <v>2.057</v>
       </c>
       <c r="C29">
         <v>1</v>
       </c>
       <c r="D29">
-        <v>0.4211479346681947</v>
+        <v>0.656</v>
       </c>
       <c r="E29">
-        <v>0.5296808495389077</v>
+        <v>0.439</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -971,10 +971,10 @@
         <v>32</v>
       </c>
       <c r="B30">
-        <v>693.4190258437507</v>
+        <v>28.199</v>
       </c>
       <c r="C30">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>